<commit_message>
New Commit: Updates Excel
</commit_message>
<xml_diff>
--- a/HashTableDoubleHashingPerformanceData.xlsx
+++ b/HashTableDoubleHashingPerformanceData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\228800\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\228800\IdeaProjects\HashTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -999,7 +999,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Get Good Time</a:t>
+              <a:t>Get Successful Time</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1377,7 +1377,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Get Bad Time</a:t>
+              <a:t>Get Unsuccessful Time</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2088,6 +2088,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Get Successful Probes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2441,6 +2466,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Get Unsuccessful Probes</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6636,7 +6686,7 @@
   <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="P80" sqref="P80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>